<commit_message>
Forgot to commit spreadsheet.
</commit_message>
<xml_diff>
--- a/data/test480_Serial.xlsx
+++ b/data/test480_Serial.xlsx
@@ -46,13 +46,13 @@
     <t xml:space="preserve">Main_Loop</t>
   </si>
   <si>
+    <t xml:space="preserve">Full_Frame</t>
+  </si>
+  <si>
     <t xml:space="preserve">DrawFeatures_binary</t>
   </si>
   <si>
     <t xml:space="preserve">DrawFeatures_markers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full_Frame</t>
   </si>
   <si>
     <t xml:space="preserve">GetCenter</t>
@@ -101,6 +101,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -122,6 +123,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,10 +206,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -216,13 +218,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.89"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -334,13 +336,13 @@
         <v>25.58957141</v>
       </c>
       <c r="C6" s="2" t="n">
+        <v>25.58501194</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>0.13305706</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="E6" s="2" t="n">
         <v>0.13728489</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>25.58501194</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.1482694</v>
@@ -362,6 +364,10 @@
       </c>
       <c r="L6" s="2" t="n">
         <v>8.333769857</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">SUM(D6:L6)</f>
+        <v>17.742512725</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,13 +378,13 @@
         <v>25.058957141</v>
       </c>
       <c r="C7" s="2" t="n">
+        <v>9.7664E-005</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>2.2213E-005</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="E7" s="2" t="n">
         <v>2.2919E-005</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>9.7664E-005</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2.4752E-005</v>
@@ -401,105 +407,157 @@
       <c r="L7" s="2" t="n">
         <v>0.000557211</v>
       </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">SUM(D7:L7)</f>
+        <v>0.001576277</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">C6/C9</f>
+        <v>0.0427128746911519</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">D6/D9</f>
+        <v>0.000222131986644407</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">E6/E9</f>
+        <v>0.000229190133555927</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">F6/F9</f>
+        <v>0.000247528213689482</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">G6/G9</f>
+        <v>0.000189850123539232</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">H6/H9</f>
+        <v>0.0103347221686144</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">I6/I9</f>
+        <v>0.000177613397328881</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">J6/J9</f>
+        <v>0.00154788883138564</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">K6/K9</f>
+        <v>0.00275849228714524</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>599</v>
+        <f aca="false">L6/L9</f>
+        <v>0.0139128044357262</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false">SUM(D8:L8)</f>
+        <v>0.0296202215776294</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B10" s="3" t="n">
         <f aca="false">B6/B6</f>
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="C10" s="4" t="n">
         <f aca="false">C6/B6</f>
+        <v>0.99982182311978</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <f aca="false">D6/B6</f>
         <v>0.00519965957491587</v>
       </c>
-      <c r="D9" s="4" t="n">
-        <f aca="false">D6/B6</f>
+      <c r="E10" s="4" t="n">
+        <f aca="false">E6/B6</f>
         <v>0.00536487648817562</v>
       </c>
-      <c r="E9" s="4" t="n">
-        <f aca="false">E6/B6</f>
-        <v>0.99982182311978</v>
-      </c>
-      <c r="F9" s="4" t="n">
+      <c r="F10" s="4" t="n">
         <f aca="false">F6/B6</f>
         <v>0.00579413377521667</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G10" s="4" t="n">
         <f aca="false">G6/B6</f>
         <v>0.00444400659073016</v>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="H10" s="4" t="n">
         <f aca="false">H6/B6</f>
         <v>0.241914898839644</v>
       </c>
-      <c r="I9" s="4" t="n">
+      <c r="I10" s="4" t="n">
         <f aca="false">I6/B6</f>
         <v>0.00415756963238643</v>
       </c>
-      <c r="J9" s="4" t="n">
+      <c r="J10" s="4" t="n">
         <f aca="false">J6/B6</f>
         <v>0.0362329401749054</v>
       </c>
-      <c r="K9" s="4" t="n">
+      <c r="K10" s="4" t="n">
         <f aca="false">K6/B6</f>
         <v>0.0645707133396651</v>
       </c>
-      <c r="L9" s="2" t="n">
+      <c r="L10" s="2" t="n">
         <f aca="false">L6/B6</f>
         <v>0.325670552408834</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H10" s="0" t="n">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L11" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>